<commit_message>
change auto collect check database
</commit_message>
<xml_diff>
--- a/database/industries/folad/folad/product/monthly_seprated.xlsx
+++ b/database/industries/folad/folad/product/monthly_seprated.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\folad\folad\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB200A82-2690-4D47-A17B-0FB390BA8D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="88">
   <si>
     <t>Pouya Finance</t>
   </si>
@@ -35,9 +34,6 @@
   </si>
   <si>
     <t>مقدار تولید</t>
-  </si>
-  <si>
-    <t>ماه 6 منتهی به 1397/06</t>
   </si>
   <si>
     <t>ماه 7 منتهی به 1397/07</t>
@@ -187,6 +183,9 @@
     <t>ماه 7 منتهی به 1401/07</t>
   </si>
   <si>
+    <t>ماه 8 منتهی به 1401/08</t>
+  </si>
+  <si>
     <t>مقدار تولید داخلی</t>
   </si>
   <si>
@@ -289,7 +288,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,7 +475,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -488,7 +487,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -535,23 +534,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -587,23 +569,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -755,17 +720,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BB91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="54" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -820,7 +785,7 @@
       <c r="BA1" s="1"/>
       <c r="BB1" s="1"/>
     </row>
-    <row r="2" spans="2:54" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:54" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -877,7 +842,7 @@
       <c r="BA2" s="1"/>
       <c r="BB2" s="1"/>
     </row>
-    <row r="3" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -934,7 +899,7 @@
       <c r="BA3" s="1"/>
       <c r="BB3" s="1"/>
     </row>
-    <row r="4" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -989,7 +954,7 @@
       <c r="BA4" s="1"/>
       <c r="BB4" s="1"/>
     </row>
-    <row r="5" spans="2:54" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="5" spans="2:54" ht="42" x14ac:dyDescent="0.65">
       <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1046,7 +1011,7 @@
       <c r="BA5" s="4"/>
       <c r="BB5" s="4"/>
     </row>
-    <row r="6" spans="2:54" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="6" spans="2:54" ht="42" x14ac:dyDescent="0.65">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1103,7 +1068,7 @@
       <c r="BA6" s="4"/>
       <c r="BB6" s="4"/>
     </row>
-    <row r="7" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1158,7 +1123,7 @@
       <c r="BA7" s="1"/>
       <c r="BB7" s="1"/>
     </row>
-    <row r="8" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1315,7 +1280,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1370,7 +1335,7 @@
       <c r="BA9" s="1"/>
       <c r="BB9" s="1"/>
     </row>
-    <row r="10" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>55</v>
       </c>
@@ -1427,7 +1392,7 @@
       <c r="BA10" s="9"/>
       <c r="BB10" s="9"/>
     </row>
-    <row r="11" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>56</v>
       </c>
@@ -1498,95 +1463,95 @@
       <c r="Y11" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z11" s="11" t="s">
-        <v>58</v>
+      <c r="Z11" s="11">
+        <v>124</v>
       </c>
       <c r="AA11" s="11">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="AB11" s="11">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="AC11" s="11">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="AD11" s="11">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="AE11" s="11">
-        <v>156</v>
+        <v>104</v>
       </c>
       <c r="AF11" s="11">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="AG11" s="11">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="AH11" s="11">
-        <v>87</v>
+        <v>195</v>
       </c>
       <c r="AI11" s="11">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="AJ11" s="11">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="AK11" s="11">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="AL11" s="11">
-        <v>165</v>
+        <v>73</v>
       </c>
       <c r="AM11" s="11">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="AN11" s="11">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="AO11" s="11">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="AP11" s="11">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="AQ11" s="11">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="AR11" s="11">
-        <v>59</v>
-      </c>
-      <c r="AS11" s="11">
         <v>81</v>
       </c>
-      <c r="AT11" s="11">
-        <v>191</v>
-      </c>
-      <c r="AU11" s="11" t="s">
-        <v>58</v>
+      <c r="AS11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU11" s="11">
+        <v>228</v>
       </c>
       <c r="AV11" s="11">
-        <v>228</v>
+        <v>107</v>
       </c>
       <c r="AW11" s="11">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="AX11" s="11">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AY11" s="11">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="AZ11" s="11">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="BA11" s="11">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="BB11" s="11">
-        <v>133</v>
+        <v>170</v>
       </c>
     </row>
-    <row r="12" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>59</v>
       </c>
@@ -1657,95 +1622,95 @@
       <c r="Y12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z12" s="13" t="s">
-        <v>58</v>
+      <c r="Z12" s="13">
+        <v>392</v>
       </c>
       <c r="AA12" s="13">
-        <v>392</v>
+        <v>368</v>
       </c>
       <c r="AB12" s="13">
-        <v>368</v>
+        <v>412</v>
       </c>
       <c r="AC12" s="13">
-        <v>412</v>
+        <v>309</v>
       </c>
       <c r="AD12" s="13">
-        <v>309</v>
+        <v>358</v>
       </c>
       <c r="AE12" s="13">
-        <v>358</v>
+        <v>288</v>
       </c>
       <c r="AF12" s="13">
+        <v>364</v>
+      </c>
+      <c r="AG12" s="13">
+        <v>381</v>
+      </c>
+      <c r="AH12" s="13">
+        <v>402</v>
+      </c>
+      <c r="AI12" s="13">
+        <v>407</v>
+      </c>
+      <c r="AJ12" s="13">
+        <v>457</v>
+      </c>
+      <c r="AK12" s="13">
         <v>288</v>
       </c>
-      <c r="AG12" s="13">
-        <v>364</v>
-      </c>
-      <c r="AH12" s="13">
-        <v>381</v>
-      </c>
-      <c r="AI12" s="13">
-        <v>402</v>
-      </c>
-      <c r="AJ12" s="13">
-        <v>407</v>
-      </c>
-      <c r="AK12" s="13">
-        <v>457</v>
-      </c>
       <c r="AL12" s="13">
-        <v>288</v>
+        <v>234</v>
       </c>
       <c r="AM12" s="13">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="AN12" s="13">
-        <v>222</v>
+        <v>323</v>
       </c>
       <c r="AO12" s="13">
-        <v>323</v>
+        <v>342</v>
       </c>
       <c r="AP12" s="13">
-        <v>342</v>
+        <v>386</v>
       </c>
       <c r="AQ12" s="13">
-        <v>386</v>
+        <v>400</v>
       </c>
       <c r="AR12" s="13">
-        <v>400</v>
+        <v>380</v>
       </c>
       <c r="AS12" s="13">
-        <v>380</v>
+        <v>1542</v>
       </c>
       <c r="AT12" s="13">
-        <v>365</v>
+        <v>555</v>
       </c>
       <c r="AU12" s="13">
-        <v>555</v>
+        <v>485</v>
       </c>
       <c r="AV12" s="13">
-        <v>485</v>
+        <v>470</v>
       </c>
       <c r="AW12" s="13">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="AX12" s="13">
-        <v>467</v>
+        <v>353</v>
       </c>
       <c r="AY12" s="13">
-        <v>353</v>
+        <v>282</v>
       </c>
       <c r="AZ12" s="13">
-        <v>282</v>
+        <v>343</v>
       </c>
       <c r="BA12" s="13">
-        <v>343</v>
+        <v>396</v>
       </c>
       <c r="BB12" s="13">
-        <v>395</v>
+        <v>415</v>
       </c>
     </row>
-    <row r="13" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>60</v>
       </c>
@@ -1816,95 +1781,95 @@
       <c r="Y13" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z13" s="11" t="s">
-        <v>58</v>
+      <c r="Z13" s="11">
+        <v>24</v>
       </c>
       <c r="AA13" s="11">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AB13" s="11">
+        <v>26</v>
+      </c>
+      <c r="AC13" s="11">
         <v>25</v>
       </c>
-      <c r="AC13" s="11">
+      <c r="AD13" s="11">
         <v>26</v>
       </c>
-      <c r="AD13" s="11">
+      <c r="AE13" s="11">
+        <v>30</v>
+      </c>
+      <c r="AF13" s="11">
         <v>25</v>
-      </c>
-      <c r="AE13" s="11">
-        <v>26</v>
-      </c>
-      <c r="AF13" s="11">
-        <v>30</v>
       </c>
       <c r="AG13" s="11">
         <v>25</v>
       </c>
       <c r="AH13" s="11">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="AI13" s="11">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="AJ13" s="11">
+        <v>27</v>
+      </c>
+      <c r="AK13" s="11">
         <v>26</v>
-      </c>
-      <c r="AK13" s="11">
-        <v>27</v>
       </c>
       <c r="AL13" s="11">
         <v>26</v>
       </c>
       <c r="AM13" s="11">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="AN13" s="11">
+        <v>28</v>
+      </c>
+      <c r="AO13" s="11">
+        <v>25</v>
+      </c>
+      <c r="AP13" s="11">
         <v>24</v>
       </c>
-      <c r="AO13" s="11">
-        <v>28</v>
-      </c>
-      <c r="AP13" s="11">
+      <c r="AQ13" s="11">
         <v>25</v>
       </c>
-      <c r="AQ13" s="11">
+      <c r="AR13" s="11">
+        <v>29</v>
+      </c>
+      <c r="AS13" s="11">
+        <v>32</v>
+      </c>
+      <c r="AT13" s="11">
+        <v>31</v>
+      </c>
+      <c r="AU13" s="11">
+        <v>29</v>
+      </c>
+      <c r="AV13" s="11">
+        <v>34</v>
+      </c>
+      <c r="AW13" s="11">
+        <v>31</v>
+      </c>
+      <c r="AX13" s="11">
         <v>24</v>
       </c>
-      <c r="AR13" s="11">
-        <v>25</v>
-      </c>
-      <c r="AS13" s="11">
-        <v>29</v>
-      </c>
-      <c r="AT13" s="11">
-        <v>32</v>
-      </c>
-      <c r="AU13" s="11">
-        <v>31</v>
-      </c>
-      <c r="AV13" s="11">
-        <v>29</v>
-      </c>
-      <c r="AW13" s="11">
-        <v>34</v>
-      </c>
-      <c r="AX13" s="11">
-        <v>31</v>
-      </c>
       <c r="AY13" s="11">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="AZ13" s="11">
+        <v>19</v>
+      </c>
+      <c r="BA13" s="11">
+        <v>20</v>
+      </c>
+      <c r="BB13" s="11">
         <v>21</v>
       </c>
-      <c r="BA13" s="11">
-        <v>19</v>
-      </c>
-      <c r="BB13" s="11">
-        <v>20</v>
-      </c>
     </row>
-    <row r="14" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
         <v>61</v>
       </c>
@@ -1975,95 +1940,95 @@
       <c r="Y14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z14" s="13" t="s">
-        <v>58</v>
+      <c r="Z14" s="13">
+        <v>134</v>
       </c>
       <c r="AA14" s="13">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="AB14" s="13">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AC14" s="13">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AD14" s="13">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="AE14" s="13">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="AF14" s="13">
         <v>123</v>
       </c>
       <c r="AG14" s="13">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="AH14" s="13">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="AI14" s="13">
+        <v>119</v>
+      </c>
+      <c r="AJ14" s="13">
+        <v>130</v>
+      </c>
+      <c r="AK14" s="13">
+        <v>119</v>
+      </c>
+      <c r="AL14" s="13">
         <v>116</v>
       </c>
-      <c r="AJ14" s="13">
+      <c r="AM14" s="13">
+        <v>128</v>
+      </c>
+      <c r="AN14" s="13">
+        <v>130</v>
+      </c>
+      <c r="AO14" s="13">
         <v>119</v>
       </c>
-      <c r="AK14" s="13">
-        <v>130</v>
-      </c>
-      <c r="AL14" s="13">
+      <c r="AP14" s="13">
+        <v>124</v>
+      </c>
+      <c r="AQ14" s="13">
+        <v>133</v>
+      </c>
+      <c r="AR14" s="13">
+        <v>120</v>
+      </c>
+      <c r="AS14" s="13">
+        <v>128</v>
+      </c>
+      <c r="AT14" s="13">
+        <v>120</v>
+      </c>
+      <c r="AU14" s="13">
+        <v>126</v>
+      </c>
+      <c r="AV14" s="13">
+        <v>124</v>
+      </c>
+      <c r="AW14" s="13">
         <v>119</v>
       </c>
-      <c r="AM14" s="13">
-        <v>116</v>
-      </c>
-      <c r="AN14" s="13">
-        <v>128</v>
-      </c>
-      <c r="AO14" s="13">
-        <v>130</v>
-      </c>
-      <c r="AP14" s="13">
-        <v>119</v>
-      </c>
-      <c r="AQ14" s="13">
-        <v>124</v>
-      </c>
-      <c r="AR14" s="13">
-        <v>133</v>
-      </c>
-      <c r="AS14" s="13">
+      <c r="AX14" s="13">
+        <v>108</v>
+      </c>
+      <c r="AY14" s="13">
+        <v>132</v>
+      </c>
+      <c r="AZ14" s="13">
         <v>120</v>
       </c>
-      <c r="AT14" s="13">
-        <v>128</v>
-      </c>
-      <c r="AU14" s="13">
-        <v>120</v>
-      </c>
-      <c r="AV14" s="13">
-        <v>126</v>
-      </c>
-      <c r="AW14" s="13">
-        <v>124</v>
-      </c>
-      <c r="AX14" s="13">
-        <v>119</v>
-      </c>
-      <c r="AY14" s="13">
-        <v>108</v>
-      </c>
-      <c r="AZ14" s="13">
-        <v>132</v>
-      </c>
       <c r="BA14" s="13">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="BB14" s="13">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
-    <row r="15" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>62</v>
       </c>
@@ -2133,94 +2098,94 @@
         <v>0</v>
       </c>
       <c r="Z15" s="15">
-        <v>0</v>
+        <v>674</v>
       </c>
       <c r="AA15" s="15">
-        <v>674</v>
+        <v>613</v>
       </c>
       <c r="AB15" s="15">
-        <v>613</v>
+        <v>723</v>
       </c>
       <c r="AC15" s="15">
-        <v>723</v>
+        <v>620</v>
       </c>
       <c r="AD15" s="15">
-        <v>620</v>
+        <v>659</v>
       </c>
       <c r="AE15" s="15">
-        <v>659</v>
+        <v>545</v>
       </c>
       <c r="AF15" s="15">
-        <v>545</v>
+        <v>594</v>
       </c>
       <c r="AG15" s="15">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="AH15" s="15">
-        <v>603</v>
+        <v>735</v>
       </c>
       <c r="AI15" s="15">
+        <v>755</v>
+      </c>
+      <c r="AJ15" s="15">
+        <v>822</v>
+      </c>
+      <c r="AK15" s="15">
+        <v>598</v>
+      </c>
+      <c r="AL15" s="15">
+        <v>449</v>
+      </c>
+      <c r="AM15" s="15">
+        <v>398</v>
+      </c>
+      <c r="AN15" s="15">
+        <v>559</v>
+      </c>
+      <c r="AO15" s="15">
+        <v>490</v>
+      </c>
+      <c r="AP15" s="15">
+        <v>601</v>
+      </c>
+      <c r="AQ15" s="15">
+        <v>617</v>
+      </c>
+      <c r="AR15" s="15">
+        <v>610</v>
+      </c>
+      <c r="AS15" s="15">
+        <v>1702</v>
+      </c>
+      <c r="AT15" s="15">
+        <v>706</v>
+      </c>
+      <c r="AU15" s="15">
+        <v>868</v>
+      </c>
+      <c r="AV15" s="15">
         <v>735</v>
       </c>
-      <c r="AJ15" s="15">
-        <v>755</v>
-      </c>
-      <c r="AK15" s="15">
-        <v>822</v>
-      </c>
-      <c r="AL15" s="15">
-        <v>598</v>
-      </c>
-      <c r="AM15" s="15">
-        <v>449</v>
-      </c>
-      <c r="AN15" s="15">
-        <v>398</v>
-      </c>
-      <c r="AO15" s="15">
-        <v>559</v>
-      </c>
-      <c r="AP15" s="15">
-        <v>490</v>
-      </c>
-      <c r="AQ15" s="15">
-        <v>601</v>
-      </c>
-      <c r="AR15" s="15">
-        <v>617</v>
-      </c>
-      <c r="AS15" s="15">
-        <v>610</v>
-      </c>
-      <c r="AT15" s="15">
-        <v>716</v>
-      </c>
-      <c r="AU15" s="15">
-        <v>706</v>
-      </c>
-      <c r="AV15" s="15">
-        <v>868</v>
-      </c>
       <c r="AW15" s="15">
-        <v>735</v>
+        <v>709</v>
       </c>
       <c r="AX15" s="15">
-        <v>709</v>
+        <v>585</v>
       </c>
       <c r="AY15" s="15">
-        <v>585</v>
+        <v>500</v>
       </c>
       <c r="AZ15" s="15">
-        <v>500</v>
+        <v>645</v>
       </c>
       <c r="BA15" s="15">
-        <v>645</v>
+        <v>667</v>
       </c>
       <c r="BB15" s="15">
-        <v>666</v>
+        <v>727</v>
       </c>
     </row>
-    <row r="16" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>63</v>
       </c>
@@ -2277,7 +2242,7 @@
       <c r="BA16" s="9"/>
       <c r="BB16" s="9"/>
     </row>
-    <row r="17" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>56</v>
       </c>
@@ -2348,8 +2313,8 @@
       <c r="Y17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z17" s="11" t="s">
-        <v>58</v>
+      <c r="Z17" s="11">
+        <v>0</v>
       </c>
       <c r="AA17" s="11">
         <v>0</v>
@@ -2375,8 +2340,8 @@
       <c r="AH17" s="11">
         <v>0</v>
       </c>
-      <c r="AI17" s="11">
-        <v>0</v>
+      <c r="AI17" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ17" s="11" t="s">
         <v>58</v>
@@ -2411,8 +2376,8 @@
       <c r="AT17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AU17" s="11" t="s">
-        <v>58</v>
+      <c r="AU17" s="11">
+        <v>0</v>
       </c>
       <c r="AV17" s="11">
         <v>0</v>
@@ -2436,7 +2401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>59</v>
       </c>
@@ -2507,8 +2472,8 @@
       <c r="Y18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z18" s="13" t="s">
-        <v>58</v>
+      <c r="Z18" s="13">
+        <v>0</v>
       </c>
       <c r="AA18" s="13">
         <v>0</v>
@@ -2534,8 +2499,8 @@
       <c r="AH18" s="13">
         <v>0</v>
       </c>
-      <c r="AI18" s="13">
-        <v>0</v>
+      <c r="AI18" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="AJ18" s="13" t="s">
         <v>58</v>
@@ -2564,14 +2529,14 @@
       <c r="AR18" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AS18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT18" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU18" s="13" t="s">
-        <v>58</v>
+      <c r="AS18" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="13">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="13">
+        <v>0</v>
       </c>
       <c r="AV18" s="13">
         <v>0</v>
@@ -2595,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>60</v>
       </c>
@@ -2666,8 +2631,8 @@
       <c r="Y19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z19" s="11" t="s">
-        <v>58</v>
+      <c r="Z19" s="11">
+        <v>0</v>
       </c>
       <c r="AA19" s="11">
         <v>0</v>
@@ -2693,8 +2658,8 @@
       <c r="AH19" s="11">
         <v>0</v>
       </c>
-      <c r="AI19" s="11">
-        <v>0</v>
+      <c r="AI19" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ19" s="11" t="s">
         <v>58</v>
@@ -2723,14 +2688,14 @@
       <c r="AR19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AS19" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT19" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU19" s="11" t="s">
-        <v>58</v>
+      <c r="AS19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="11">
+        <v>0</v>
       </c>
       <c r="AV19" s="11">
         <v>0</v>
@@ -2754,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>61</v>
       </c>
@@ -2825,8 +2790,8 @@
       <c r="Y20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z20" s="13" t="s">
-        <v>58</v>
+      <c r="Z20" s="13">
+        <v>0</v>
       </c>
       <c r="AA20" s="13">
         <v>0</v>
@@ -2852,8 +2817,8 @@
       <c r="AH20" s="13">
         <v>0</v>
       </c>
-      <c r="AI20" s="13">
-        <v>0</v>
+      <c r="AI20" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="AJ20" s="13" t="s">
         <v>58</v>
@@ -2882,14 +2847,14 @@
       <c r="AR20" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AS20" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT20" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AU20" s="13" t="s">
-        <v>58</v>
+      <c r="AS20" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="13">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="13">
+        <v>0</v>
       </c>
       <c r="AV20" s="13">
         <v>0</v>
@@ -2913,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>64</v>
       </c>
@@ -3070,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
         <v>65</v>
       </c>
@@ -3127,7 +3092,7 @@
       <c r="BA22" s="9"/>
       <c r="BB22" s="9"/>
     </row>
-    <row r="23" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>56</v>
       </c>
@@ -3198,8 +3163,8 @@
       <c r="Y23" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z23" s="11" t="s">
-        <v>58</v>
+      <c r="Z23" s="11">
+        <v>0</v>
       </c>
       <c r="AA23" s="11">
         <v>0</v>
@@ -3225,8 +3190,8 @@
       <c r="AH23" s="11">
         <v>0</v>
       </c>
-      <c r="AI23" s="11">
-        <v>0</v>
+      <c r="AI23" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ23" s="11" t="s">
         <v>58</v>
@@ -3286,7 +3251,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>66</v>
       </c>
@@ -3355,8 +3320,8 @@
       <c r="Y24" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Z24" s="17" t="s">
-        <v>58</v>
+      <c r="Z24" s="17">
+        <v>0</v>
       </c>
       <c r="AA24" s="17">
         <v>0</v>
@@ -3443,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>67</v>
       </c>
@@ -3513,94 +3478,94 @@
         <v>0</v>
       </c>
       <c r="Z25" s="15">
-        <v>0</v>
+        <v>674</v>
       </c>
       <c r="AA25" s="15">
-        <v>674</v>
+        <v>613</v>
       </c>
       <c r="AB25" s="15">
-        <v>613</v>
+        <v>723</v>
       </c>
       <c r="AC25" s="15">
-        <v>723</v>
+        <v>620</v>
       </c>
       <c r="AD25" s="15">
-        <v>620</v>
+        <v>659</v>
       </c>
       <c r="AE25" s="15">
-        <v>659</v>
+        <v>545</v>
       </c>
       <c r="AF25" s="15">
-        <v>545</v>
+        <v>594</v>
       </c>
       <c r="AG25" s="15">
-        <v>594</v>
+        <v>603</v>
       </c>
       <c r="AH25" s="15">
-        <v>603</v>
+        <v>735</v>
       </c>
       <c r="AI25" s="15">
+        <v>755</v>
+      </c>
+      <c r="AJ25" s="15">
+        <v>822</v>
+      </c>
+      <c r="AK25" s="15">
+        <v>598</v>
+      </c>
+      <c r="AL25" s="15">
+        <v>449</v>
+      </c>
+      <c r="AM25" s="15">
+        <v>398</v>
+      </c>
+      <c r="AN25" s="15">
+        <v>559</v>
+      </c>
+      <c r="AO25" s="15">
+        <v>490</v>
+      </c>
+      <c r="AP25" s="15">
+        <v>601</v>
+      </c>
+      <c r="AQ25" s="15">
+        <v>617</v>
+      </c>
+      <c r="AR25" s="15">
+        <v>610</v>
+      </c>
+      <c r="AS25" s="15">
+        <v>1702</v>
+      </c>
+      <c r="AT25" s="15">
+        <v>706</v>
+      </c>
+      <c r="AU25" s="15">
+        <v>868</v>
+      </c>
+      <c r="AV25" s="15">
         <v>735</v>
       </c>
-      <c r="AJ25" s="15">
-        <v>755</v>
-      </c>
-      <c r="AK25" s="15">
-        <v>822</v>
-      </c>
-      <c r="AL25" s="15">
-        <v>598</v>
-      </c>
-      <c r="AM25" s="15">
-        <v>449</v>
-      </c>
-      <c r="AN25" s="15">
-        <v>398</v>
-      </c>
-      <c r="AO25" s="15">
-        <v>559</v>
-      </c>
-      <c r="AP25" s="15">
-        <v>490</v>
-      </c>
-      <c r="AQ25" s="15">
-        <v>601</v>
-      </c>
-      <c r="AR25" s="15">
-        <v>617</v>
-      </c>
-      <c r="AS25" s="15">
-        <v>610</v>
-      </c>
-      <c r="AT25" s="15">
-        <v>716</v>
-      </c>
-      <c r="AU25" s="15">
-        <v>706</v>
-      </c>
-      <c r="AV25" s="15">
-        <v>868</v>
-      </c>
       <c r="AW25" s="15">
-        <v>735</v>
+        <v>709</v>
       </c>
       <c r="AX25" s="15">
-        <v>709</v>
+        <v>585</v>
       </c>
       <c r="AY25" s="15">
-        <v>585</v>
+        <v>500</v>
       </c>
       <c r="AZ25" s="15">
-        <v>500</v>
+        <v>645</v>
       </c>
       <c r="BA25" s="15">
-        <v>645</v>
+        <v>667</v>
       </c>
       <c r="BB25" s="15">
-        <v>666</v>
+        <v>727</v>
       </c>
     </row>
-    <row r="26" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -3655,7 +3620,7 @@
       <c r="BA26" s="1"/>
       <c r="BB26" s="1"/>
     </row>
-    <row r="27" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -3710,7 +3675,7 @@
       <c r="BA27" s="1"/>
       <c r="BB27" s="1"/>
     </row>
-    <row r="28" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -3765,7 +3730,7 @@
       <c r="BA28" s="1"/>
       <c r="BB28" s="1"/>
     </row>
-    <row r="29" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>68</v>
       </c>
@@ -3922,7 +3887,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -3977,7 +3942,7 @@
       <c r="BA30" s="1"/>
       <c r="BB30" s="1"/>
     </row>
-    <row r="31" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B31" s="8" t="s">
         <v>69</v>
       </c>
@@ -4034,7 +3999,7 @@
       <c r="BA31" s="9"/>
       <c r="BB31" s="9"/>
     </row>
-    <row r="32" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B32" s="10" t="s">
         <v>56</v>
       </c>
@@ -4105,95 +4070,95 @@
       <c r="Y32" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z32" s="11" t="s">
-        <v>58</v>
+      <c r="Z32" s="11">
+        <v>125</v>
       </c>
       <c r="AA32" s="11">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="AB32" s="11">
+        <v>84</v>
+      </c>
+      <c r="AC32" s="11">
+        <v>92</v>
+      </c>
+      <c r="AD32" s="11">
+        <v>172</v>
+      </c>
+      <c r="AE32" s="11">
+        <v>122</v>
+      </c>
+      <c r="AF32" s="11">
+        <v>137</v>
+      </c>
+      <c r="AG32" s="11">
+        <v>101</v>
+      </c>
+      <c r="AH32" s="11">
+        <v>138</v>
+      </c>
+      <c r="AI32" s="11">
+        <v>56</v>
+      </c>
+      <c r="AJ32" s="11">
+        <v>191</v>
+      </c>
+      <c r="AK32" s="11">
+        <v>233</v>
+      </c>
+      <c r="AL32" s="11">
+        <v>159</v>
+      </c>
+      <c r="AM32" s="11">
+        <v>59</v>
+      </c>
+      <c r="AN32" s="11">
+        <v>80</v>
+      </c>
+      <c r="AO32" s="11">
+        <v>129</v>
+      </c>
+      <c r="AP32" s="11">
         <v>62</v>
       </c>
-      <c r="AC32" s="11">
-        <v>84</v>
-      </c>
-      <c r="AD32" s="11">
-        <v>92</v>
-      </c>
-      <c r="AE32" s="11">
+      <c r="AQ32" s="11">
+        <v>91</v>
+      </c>
+      <c r="AR32" s="11">
+        <v>69</v>
+      </c>
+      <c r="AS32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU32" s="11">
+        <v>67</v>
+      </c>
+      <c r="AV32" s="11">
         <v>172</v>
       </c>
-      <c r="AF32" s="11">
-        <v>122</v>
-      </c>
-      <c r="AG32" s="11">
-        <v>137</v>
-      </c>
-      <c r="AH32" s="11">
-        <v>101</v>
-      </c>
-      <c r="AI32" s="11">
-        <v>138</v>
-      </c>
-      <c r="AJ32" s="11">
-        <v>56</v>
-      </c>
-      <c r="AK32" s="11">
-        <v>191</v>
-      </c>
-      <c r="AL32" s="11">
-        <v>233</v>
-      </c>
-      <c r="AM32" s="11">
-        <v>159</v>
-      </c>
-      <c r="AN32" s="11">
-        <v>59</v>
-      </c>
-      <c r="AO32" s="11">
-        <v>80</v>
-      </c>
-      <c r="AP32" s="11">
-        <v>129</v>
-      </c>
-      <c r="AQ32" s="11">
-        <v>62</v>
-      </c>
-      <c r="AR32" s="11">
-        <v>91</v>
-      </c>
-      <c r="AS32" s="11">
-        <v>69</v>
-      </c>
-      <c r="AT32" s="11">
-        <v>84</v>
-      </c>
-      <c r="AU32" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV32" s="11">
-        <v>67</v>
-      </c>
       <c r="AW32" s="11">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="AX32" s="11">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="AY32" s="11">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="AZ32" s="11">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="BA32" s="11">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="BB32" s="11">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
         <v>59</v>
       </c>
@@ -4264,95 +4229,95 @@
       <c r="Y33" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z33" s="13" t="s">
-        <v>58</v>
+      <c r="Z33" s="13">
+        <v>374</v>
       </c>
       <c r="AA33" s="13">
-        <v>374</v>
+        <v>323</v>
       </c>
       <c r="AB33" s="13">
-        <v>323</v>
+        <v>388</v>
       </c>
       <c r="AC33" s="13">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="AD33" s="13">
-        <v>384</v>
+        <v>365</v>
       </c>
       <c r="AE33" s="13">
-        <v>365</v>
+        <v>322</v>
       </c>
       <c r="AF33" s="13">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="AG33" s="13">
-        <v>326</v>
+        <v>359</v>
       </c>
       <c r="AH33" s="13">
-        <v>359</v>
+        <v>454</v>
       </c>
       <c r="AI33" s="13">
-        <v>454</v>
+        <v>334</v>
       </c>
       <c r="AJ33" s="13">
-        <v>334</v>
+        <v>395</v>
       </c>
       <c r="AK33" s="13">
-        <v>395</v>
+        <v>335</v>
       </c>
       <c r="AL33" s="13">
+        <v>301</v>
+      </c>
+      <c r="AM33" s="13">
+        <v>236</v>
+      </c>
+      <c r="AN33" s="13">
+        <v>341</v>
+      </c>
+      <c r="AO33" s="13">
         <v>335</v>
       </c>
-      <c r="AM33" s="13">
-        <v>301</v>
-      </c>
-      <c r="AN33" s="13">
-        <v>236</v>
-      </c>
-      <c r="AO33" s="13">
-        <v>341</v>
-      </c>
       <c r="AP33" s="13">
-        <v>335</v>
+        <v>372</v>
       </c>
       <c r="AQ33" s="13">
-        <v>372</v>
+        <v>391</v>
       </c>
       <c r="AR33" s="13">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="AS33" s="13">
-        <v>398</v>
+        <v>577</v>
       </c>
       <c r="AT33" s="13">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c r="AU33" s="13">
-        <v>400</v>
+        <v>371</v>
       </c>
       <c r="AV33" s="13">
-        <v>371</v>
+        <v>459</v>
       </c>
       <c r="AW33" s="13">
-        <v>459</v>
+        <v>523</v>
       </c>
       <c r="AX33" s="13">
-        <v>523</v>
+        <v>387</v>
       </c>
       <c r="AY33" s="13">
-        <v>387</v>
+        <v>315</v>
       </c>
       <c r="AZ33" s="13">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="BA33" s="13">
-        <v>297</v>
+        <v>358</v>
       </c>
       <c r="BB33" s="13">
-        <v>359</v>
+        <v>380</v>
       </c>
     </row>
-    <row r="34" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B34" s="10" t="s">
         <v>60</v>
       </c>
@@ -4423,95 +4388,95 @@
       <c r="Y34" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z34" s="11" t="s">
-        <v>58</v>
+      <c r="Z34" s="11">
+        <v>28</v>
       </c>
       <c r="AA34" s="11">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB34" s="11">
         <v>27</v>
       </c>
       <c r="AC34" s="11">
+        <v>38</v>
+      </c>
+      <c r="AD34" s="11">
+        <v>25</v>
+      </c>
+      <c r="AE34" s="11">
+        <v>29</v>
+      </c>
+      <c r="AF34" s="11">
+        <v>37</v>
+      </c>
+      <c r="AG34" s="11">
+        <v>25</v>
+      </c>
+      <c r="AH34" s="11">
+        <v>22</v>
+      </c>
+      <c r="AI34" s="11">
+        <v>25</v>
+      </c>
+      <c r="AJ34" s="11">
+        <v>26</v>
+      </c>
+      <c r="AK34" s="11">
+        <v>29</v>
+      </c>
+      <c r="AL34" s="11">
         <v>27</v>
       </c>
-      <c r="AD34" s="11">
-        <v>38</v>
-      </c>
-      <c r="AE34" s="11">
+      <c r="AM34" s="11">
         <v>25</v>
-      </c>
-      <c r="AF34" s="11">
-        <v>29</v>
-      </c>
-      <c r="AG34" s="11">
-        <v>37</v>
-      </c>
-      <c r="AH34" s="11">
-        <v>25</v>
-      </c>
-      <c r="AI34" s="11">
-        <v>22</v>
-      </c>
-      <c r="AJ34" s="11">
-        <v>25</v>
-      </c>
-      <c r="AK34" s="11">
-        <v>26</v>
-      </c>
-      <c r="AL34" s="11">
-        <v>29</v>
-      </c>
-      <c r="AM34" s="11">
-        <v>27</v>
       </c>
       <c r="AN34" s="11">
         <v>25</v>
       </c>
       <c r="AO34" s="11">
+        <v>20</v>
+      </c>
+      <c r="AP34" s="11">
         <v>25</v>
-      </c>
-      <c r="AP34" s="11">
-        <v>20</v>
       </c>
       <c r="AQ34" s="11">
         <v>25</v>
       </c>
       <c r="AR34" s="11">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="AS34" s="11">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="AT34" s="11">
+        <v>29</v>
+      </c>
+      <c r="AU34" s="11">
+        <v>24</v>
+      </c>
+      <c r="AV34" s="11">
         <v>30</v>
       </c>
-      <c r="AU34" s="11">
-        <v>29</v>
-      </c>
-      <c r="AV34" s="11">
-        <v>24</v>
-      </c>
       <c r="AW34" s="11">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AX34" s="11">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="AY34" s="11">
         <v>23</v>
       </c>
       <c r="AZ34" s="11">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="BA34" s="11">
+        <v>18</v>
+      </c>
+      <c r="BB34" s="11">
         <v>22</v>
       </c>
-      <c r="BB34" s="11">
-        <v>18</v>
-      </c>
     </row>
-    <row r="35" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
         <v>61</v>
       </c>
@@ -4582,95 +4547,95 @@
       <c r="Y35" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z35" s="13" t="s">
-        <v>58</v>
+      <c r="Z35" s="13">
+        <v>149</v>
       </c>
       <c r="AA35" s="13">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="AB35" s="13">
+        <v>120</v>
+      </c>
+      <c r="AC35" s="13">
+        <v>132</v>
+      </c>
+      <c r="AD35" s="13">
+        <v>110</v>
+      </c>
+      <c r="AE35" s="13">
+        <v>136</v>
+      </c>
+      <c r="AF35" s="13">
+        <v>125</v>
+      </c>
+      <c r="AG35" s="13">
+        <v>112</v>
+      </c>
+      <c r="AH35" s="13">
+        <v>117</v>
+      </c>
+      <c r="AI35" s="13">
+        <v>114</v>
+      </c>
+      <c r="AJ35" s="13">
+        <v>125</v>
+      </c>
+      <c r="AK35" s="13">
         <v>113</v>
       </c>
-      <c r="AC35" s="13">
+      <c r="AL35" s="13">
+        <v>125</v>
+      </c>
+      <c r="AM35" s="13">
+        <v>117</v>
+      </c>
+      <c r="AN35" s="13">
+        <v>129</v>
+      </c>
+      <c r="AO35" s="13">
         <v>120</v>
       </c>
-      <c r="AD35" s="13">
-        <v>132</v>
-      </c>
-      <c r="AE35" s="13">
-        <v>110</v>
-      </c>
-      <c r="AF35" s="13">
-        <v>136</v>
-      </c>
-      <c r="AG35" s="13">
-        <v>125</v>
-      </c>
-      <c r="AH35" s="13">
+      <c r="AP35" s="13">
+        <v>127</v>
+      </c>
+      <c r="AQ35" s="13">
+        <v>130</v>
+      </c>
+      <c r="AR35" s="13">
         <v>112</v>
       </c>
-      <c r="AI35" s="13">
-        <v>117</v>
-      </c>
-      <c r="AJ35" s="13">
-        <v>114</v>
-      </c>
-      <c r="AK35" s="13">
-        <v>125</v>
-      </c>
-      <c r="AL35" s="13">
-        <v>113</v>
-      </c>
-      <c r="AM35" s="13">
-        <v>125</v>
-      </c>
-      <c r="AN35" s="13">
-        <v>117</v>
-      </c>
-      <c r="AO35" s="13">
-        <v>129</v>
-      </c>
-      <c r="AP35" s="13">
+      <c r="AS35" s="13">
+        <v>127</v>
+      </c>
+      <c r="AT35" s="13">
         <v>120</v>
-      </c>
-      <c r="AQ35" s="13">
-        <v>127</v>
-      </c>
-      <c r="AR35" s="13">
-        <v>130</v>
-      </c>
-      <c r="AS35" s="13">
-        <v>112</v>
-      </c>
-      <c r="AT35" s="13">
-        <v>125</v>
       </c>
       <c r="AU35" s="13">
         <v>120</v>
       </c>
       <c r="AV35" s="13">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="AW35" s="13">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AX35" s="13">
+        <v>114</v>
+      </c>
+      <c r="AY35" s="13">
+        <v>108</v>
+      </c>
+      <c r="AZ35" s="13">
         <v>128</v>
       </c>
-      <c r="AY35" s="13">
-        <v>114</v>
-      </c>
-      <c r="AZ35" s="13">
-        <v>108</v>
-      </c>
       <c r="BA35" s="13">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="BB35" s="13">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="36" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
         <v>70</v>
       </c>
@@ -4740,94 +4705,94 @@
         <v>0</v>
       </c>
       <c r="Z36" s="15">
-        <v>0</v>
+        <v>676</v>
       </c>
       <c r="AA36" s="15">
-        <v>676</v>
+        <v>525</v>
       </c>
       <c r="AB36" s="15">
-        <v>525</v>
+        <v>619</v>
       </c>
       <c r="AC36" s="15">
-        <v>619</v>
+        <v>646</v>
       </c>
       <c r="AD36" s="15">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="AE36" s="15">
-        <v>672</v>
+        <v>609</v>
       </c>
       <c r="AF36" s="15">
-        <v>609</v>
+        <v>625</v>
       </c>
       <c r="AG36" s="15">
-        <v>625</v>
+        <v>597</v>
       </c>
       <c r="AH36" s="15">
-        <v>597</v>
+        <v>731</v>
       </c>
       <c r="AI36" s="15">
-        <v>731</v>
+        <v>529</v>
       </c>
       <c r="AJ36" s="15">
-        <v>529</v>
+        <v>737</v>
       </c>
       <c r="AK36" s="15">
-        <v>737</v>
+        <v>710</v>
       </c>
       <c r="AL36" s="15">
-        <v>710</v>
+        <v>612</v>
       </c>
       <c r="AM36" s="15">
-        <v>612</v>
+        <v>437</v>
       </c>
       <c r="AN36" s="15">
-        <v>437</v>
+        <v>575</v>
       </c>
       <c r="AO36" s="15">
-        <v>575</v>
+        <v>604</v>
       </c>
       <c r="AP36" s="15">
-        <v>604</v>
+        <v>586</v>
       </c>
       <c r="AQ36" s="15">
-        <v>586</v>
+        <v>637</v>
       </c>
       <c r="AR36" s="15">
-        <v>637</v>
+        <v>611</v>
       </c>
       <c r="AS36" s="15">
-        <v>611</v>
+        <v>707</v>
       </c>
       <c r="AT36" s="15">
-        <v>607</v>
+        <v>549</v>
       </c>
       <c r="AU36" s="15">
-        <v>549</v>
+        <v>582</v>
       </c>
       <c r="AV36" s="15">
-        <v>582</v>
+        <v>792</v>
       </c>
       <c r="AW36" s="15">
-        <v>792</v>
+        <v>813</v>
       </c>
       <c r="AX36" s="15">
-        <v>813</v>
+        <v>565</v>
       </c>
       <c r="AY36" s="15">
-        <v>565</v>
+        <v>475</v>
       </c>
       <c r="AZ36" s="15">
-        <v>475</v>
+        <v>492</v>
       </c>
       <c r="BA36" s="15">
-        <v>492</v>
+        <v>521</v>
       </c>
       <c r="BB36" s="15">
-        <v>522</v>
+        <v>546</v>
       </c>
     </row>
-    <row r="37" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>71</v>
       </c>
@@ -4884,7 +4849,7 @@
       <c r="BA37" s="9"/>
       <c r="BB37" s="9"/>
     </row>
-    <row r="38" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
         <v>56</v>
       </c>
@@ -4955,8 +4920,8 @@
       <c r="Y38" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z38" s="11" t="s">
-        <v>58</v>
+      <c r="Z38" s="11">
+        <v>0</v>
       </c>
       <c r="AA38" s="11">
         <v>0</v>
@@ -4982,8 +4947,8 @@
       <c r="AH38" s="11">
         <v>0</v>
       </c>
-      <c r="AI38" s="11">
-        <v>0</v>
+      <c r="AI38" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ38" s="11" t="s">
         <v>58</v>
@@ -5018,17 +4983,17 @@
       <c r="AT38" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AU38" s="11" t="s">
-        <v>58</v>
+      <c r="AU38" s="11">
+        <v>0</v>
       </c>
       <c r="AV38" s="11">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="AW38" s="11">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="AX38" s="11">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="AY38" s="11">
         <v>0</v>
@@ -5037,13 +5002,13 @@
         <v>0</v>
       </c>
       <c r="BA38" s="11">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="BB38" s="11">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="39" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
         <v>59</v>
       </c>
@@ -5114,8 +5079,8 @@
       <c r="Y39" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z39" s="13" t="s">
-        <v>58</v>
+      <c r="Z39" s="13">
+        <v>0</v>
       </c>
       <c r="AA39" s="13">
         <v>0</v>
@@ -5141,8 +5106,8 @@
       <c r="AH39" s="13">
         <v>0</v>
       </c>
-      <c r="AI39" s="13">
-        <v>0</v>
+      <c r="AI39" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="AJ39" s="13" t="s">
         <v>58</v>
@@ -5171,38 +5136,38 @@
       <c r="AR39" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AS39" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT39" s="13" t="s">
-        <v>58</v>
+      <c r="AS39" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT39" s="13">
+        <v>227</v>
       </c>
       <c r="AU39" s="13">
-        <v>227</v>
+        <v>2</v>
       </c>
       <c r="AV39" s="13">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="AW39" s="13">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="AX39" s="13">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="AY39" s="13">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="AZ39" s="13">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="BA39" s="13">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="BB39" s="13">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="40" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>60</v>
       </c>
@@ -5273,8 +5238,8 @@
       <c r="Y40" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z40" s="11" t="s">
-        <v>58</v>
+      <c r="Z40" s="11">
+        <v>0</v>
       </c>
       <c r="AA40" s="11">
         <v>0</v>
@@ -5300,8 +5265,8 @@
       <c r="AH40" s="11">
         <v>0</v>
       </c>
-      <c r="AI40" s="11">
-        <v>0</v>
+      <c r="AI40" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ40" s="11" t="s">
         <v>58</v>
@@ -5330,38 +5295,38 @@
       <c r="AR40" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AS40" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT40" s="11" t="s">
-        <v>58</v>
+      <c r="AS40" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT40" s="11">
+        <v>1</v>
       </c>
       <c r="AU40" s="11">
         <v>1</v>
       </c>
       <c r="AV40" s="11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AW40" s="11">
         <v>2</v>
       </c>
       <c r="AX40" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AY40" s="11">
         <v>1</v>
       </c>
       <c r="AZ40" s="11">
+        <v>0</v>
+      </c>
+      <c r="BA40" s="11">
+        <v>0</v>
+      </c>
+      <c r="BB40" s="11">
         <v>1</v>
       </c>
-      <c r="BA40" s="11">
-        <v>0</v>
-      </c>
-      <c r="BB40" s="11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="41" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>61</v>
       </c>
@@ -5432,8 +5397,8 @@
       <c r="Y41" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z41" s="13" t="s">
-        <v>58</v>
+      <c r="Z41" s="13">
+        <v>0</v>
       </c>
       <c r="AA41" s="13">
         <v>0</v>
@@ -5459,8 +5424,8 @@
       <c r="AH41" s="13">
         <v>0</v>
       </c>
-      <c r="AI41" s="13">
-        <v>0</v>
+      <c r="AI41" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="AJ41" s="13" t="s">
         <v>58</v>
@@ -5489,11 +5454,11 @@
       <c r="AR41" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AS41" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT41" s="13" t="s">
-        <v>58</v>
+      <c r="AS41" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT41" s="13">
+        <v>0</v>
       </c>
       <c r="AU41" s="13">
         <v>0</v>
@@ -5520,7 +5485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
         <v>72</v>
       </c>
@@ -5650,34 +5615,34 @@
         <v>0</v>
       </c>
       <c r="AT42" s="15">
-        <v>0</v>
+        <v>228</v>
       </c>
       <c r="AU42" s="15">
-        <v>228</v>
+        <v>3</v>
       </c>
       <c r="AV42" s="15">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="AW42" s="15">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="AX42" s="15">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="AY42" s="15">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="AZ42" s="15">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="BA42" s="15">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="BB42" s="15">
-        <v>42</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="43" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B43" s="8" t="s">
         <v>65</v>
       </c>
@@ -5734,7 +5699,7 @@
       <c r="BA43" s="9"/>
       <c r="BB43" s="9"/>
     </row>
-    <row r="44" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B44" s="10" t="s">
         <v>56</v>
       </c>
@@ -5805,8 +5770,8 @@
       <c r="Y44" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z44" s="11" t="s">
-        <v>58</v>
+      <c r="Z44" s="11">
+        <v>0</v>
       </c>
       <c r="AA44" s="11">
         <v>0</v>
@@ -5832,8 +5797,8 @@
       <c r="AH44" s="11">
         <v>0</v>
       </c>
-      <c r="AI44" s="11">
-        <v>0</v>
+      <c r="AI44" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ44" s="11" t="s">
         <v>58</v>
@@ -5893,7 +5858,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B45" s="16" t="s">
         <v>66</v>
       </c>
@@ -5962,8 +5927,8 @@
       <c r="Y45" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Z45" s="17" t="s">
-        <v>58</v>
+      <c r="Z45" s="17">
+        <v>0</v>
       </c>
       <c r="AA45" s="17">
         <v>0</v>
@@ -6050,7 +6015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
         <v>73</v>
       </c>
@@ -6107,7 +6072,7 @@
       <c r="BA46" s="9"/>
       <c r="BB46" s="9"/>
     </row>
-    <row r="47" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B47" s="10" t="s">
         <v>56</v>
       </c>
@@ -6178,8 +6143,8 @@
       <c r="Y47" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z47" s="11" t="s">
-        <v>58</v>
+      <c r="Z47" s="11">
+        <v>0</v>
       </c>
       <c r="AA47" s="11">
         <v>0</v>
@@ -6205,8 +6170,8 @@
       <c r="AH47" s="11">
         <v>0</v>
       </c>
-      <c r="AI47" s="11">
-        <v>0</v>
+      <c r="AI47" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ47" s="11" t="s">
         <v>58</v>
@@ -6266,7 +6231,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B48" s="16" t="s">
         <v>74</v>
       </c>
@@ -6335,8 +6300,8 @@
       <c r="Y48" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Z48" s="17" t="s">
-        <v>58</v>
+      <c r="Z48" s="17">
+        <v>0</v>
       </c>
       <c r="AA48" s="17">
         <v>0</v>
@@ -6423,7 +6388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>67</v>
       </c>
@@ -6493,94 +6458,94 @@
         <v>0</v>
       </c>
       <c r="Z49" s="15">
-        <v>0</v>
+        <v>676</v>
       </c>
       <c r="AA49" s="15">
-        <v>676</v>
+        <v>525</v>
       </c>
       <c r="AB49" s="15">
-        <v>525</v>
+        <v>619</v>
       </c>
       <c r="AC49" s="15">
-        <v>619</v>
+        <v>646</v>
       </c>
       <c r="AD49" s="15">
-        <v>646</v>
+        <v>672</v>
       </c>
       <c r="AE49" s="15">
-        <v>672</v>
+        <v>609</v>
       </c>
       <c r="AF49" s="15">
-        <v>609</v>
+        <v>625</v>
       </c>
       <c r="AG49" s="15">
-        <v>625</v>
+        <v>597</v>
       </c>
       <c r="AH49" s="15">
-        <v>597</v>
+        <v>731</v>
       </c>
       <c r="AI49" s="15">
-        <v>731</v>
+        <v>529</v>
       </c>
       <c r="AJ49" s="15">
-        <v>529</v>
+        <v>737</v>
       </c>
       <c r="AK49" s="15">
-        <v>737</v>
+        <v>710</v>
       </c>
       <c r="AL49" s="15">
-        <v>710</v>
+        <v>612</v>
       </c>
       <c r="AM49" s="15">
-        <v>612</v>
+        <v>437</v>
       </c>
       <c r="AN49" s="15">
-        <v>437</v>
+        <v>575</v>
       </c>
       <c r="AO49" s="15">
-        <v>575</v>
+        <v>604</v>
       </c>
       <c r="AP49" s="15">
-        <v>604</v>
+        <v>586</v>
       </c>
       <c r="AQ49" s="15">
-        <v>586</v>
+        <v>637</v>
       </c>
       <c r="AR49" s="15">
-        <v>637</v>
+        <v>611</v>
       </c>
       <c r="AS49" s="15">
-        <v>611</v>
+        <v>707</v>
       </c>
       <c r="AT49" s="15">
-        <v>607</v>
+        <v>777</v>
       </c>
       <c r="AU49" s="15">
-        <v>777</v>
+        <v>585</v>
       </c>
       <c r="AV49" s="15">
-        <v>585</v>
+        <v>876</v>
       </c>
       <c r="AW49" s="15">
-        <v>876</v>
+        <v>918</v>
       </c>
       <c r="AX49" s="15">
-        <v>918</v>
+        <v>574</v>
       </c>
       <c r="AY49" s="15">
-        <v>574</v>
+        <v>496</v>
       </c>
       <c r="AZ49" s="15">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="BA49" s="15">
-        <v>499</v>
+        <v>564</v>
       </c>
       <c r="BB49" s="15">
-        <v>564</v>
+        <v>633</v>
       </c>
     </row>
-    <row r="50" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -6635,7 +6600,7 @@
       <c r="BA50" s="1"/>
       <c r="BB50" s="1"/>
     </row>
-    <row r="51" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -6690,7 +6655,7 @@
       <c r="BA51" s="1"/>
       <c r="BB51" s="1"/>
     </row>
-    <row r="52" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -6745,7 +6710,7 @@
       <c r="BA52" s="1"/>
       <c r="BB52" s="1"/>
     </row>
-    <row r="53" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
         <v>75</v>
       </c>
@@ -6902,7 +6867,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -6957,7 +6922,7 @@
       <c r="BA54" s="1"/>
       <c r="BB54" s="1"/>
     </row>
-    <row r="55" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
         <v>76</v>
       </c>
@@ -7014,7 +6979,7 @@
       <c r="BA55" s="9"/>
       <c r="BB55" s="9"/>
     </row>
-    <row r="56" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>56</v>
       </c>
@@ -7085,95 +7050,95 @@
       <c r="Y56" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z56" s="11" t="s">
-        <v>58</v>
+      <c r="Z56" s="11">
+        <v>7453984</v>
       </c>
       <c r="AA56" s="11">
-        <v>7453984</v>
+        <v>4945006</v>
       </c>
       <c r="AB56" s="11">
-        <v>4945006</v>
+        <v>6238752</v>
       </c>
       <c r="AC56" s="11">
-        <v>6238752</v>
+        <v>8652238</v>
       </c>
       <c r="AD56" s="11">
-        <v>8652238</v>
+        <v>16483131</v>
       </c>
       <c r="AE56" s="11">
-        <v>16483131</v>
+        <v>14013518</v>
       </c>
       <c r="AF56" s="11">
-        <v>14013518</v>
+        <v>16872492</v>
       </c>
       <c r="AG56" s="11">
-        <v>16872492</v>
+        <v>12262783</v>
       </c>
       <c r="AH56" s="11">
-        <v>12262783</v>
+        <v>18116251</v>
       </c>
       <c r="AI56" s="11">
-        <v>18116251</v>
+        <v>7660416</v>
       </c>
       <c r="AJ56" s="11">
-        <v>7660416</v>
+        <v>25674336</v>
       </c>
       <c r="AK56" s="11">
-        <v>25674336</v>
+        <v>31520150</v>
       </c>
       <c r="AL56" s="11">
-        <v>31520150</v>
+        <v>24439925</v>
       </c>
       <c r="AM56" s="11">
-        <v>24439925</v>
+        <v>9055956</v>
       </c>
       <c r="AN56" s="11">
-        <v>9055956</v>
+        <v>12287755</v>
       </c>
       <c r="AO56" s="11">
-        <v>12287755</v>
+        <v>21394841</v>
       </c>
       <c r="AP56" s="11">
-        <v>21394841</v>
+        <v>9063719</v>
       </c>
       <c r="AQ56" s="11">
-        <v>9063719</v>
+        <v>14699295</v>
       </c>
       <c r="AR56" s="11">
-        <v>14699295</v>
-      </c>
-      <c r="AS56" s="11">
         <v>11319145</v>
       </c>
-      <c r="AT56" s="11">
-        <v>12718064</v>
-      </c>
-      <c r="AU56" s="11" t="s">
-        <v>58</v>
+      <c r="AS56" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT56" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU56" s="11">
+        <v>10550541</v>
       </c>
       <c r="AV56" s="11">
-        <v>10550541</v>
+        <v>28476840</v>
       </c>
       <c r="AW56" s="11">
-        <v>28476840</v>
+        <v>21350500</v>
       </c>
       <c r="AX56" s="11">
-        <v>21350500</v>
+        <v>8156854</v>
       </c>
       <c r="AY56" s="11">
-        <v>8156854</v>
+        <v>4269479</v>
       </c>
       <c r="AZ56" s="11">
-        <v>4269479</v>
+        <v>6967049</v>
       </c>
       <c r="BA56" s="11">
-        <v>6967049</v>
+        <v>4205447</v>
       </c>
       <c r="BB56" s="11">
-        <v>4205447</v>
+        <v>3927326</v>
       </c>
     </row>
-    <row r="57" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B57" s="12" t="s">
         <v>59</v>
       </c>
@@ -7244,95 +7209,95 @@
       <c r="Y57" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z57" s="13" t="s">
-        <v>58</v>
+      <c r="Z57" s="13">
+        <v>25065548</v>
       </c>
       <c r="AA57" s="13">
-        <v>25065548</v>
+        <v>24107939</v>
       </c>
       <c r="AB57" s="13">
-        <v>24107939</v>
+        <v>32153658</v>
       </c>
       <c r="AC57" s="13">
-        <v>32153658</v>
+        <v>36484390</v>
       </c>
       <c r="AD57" s="13">
-        <v>36484390</v>
+        <v>39571364</v>
       </c>
       <c r="AE57" s="13">
-        <v>39571364</v>
+        <v>39012934</v>
       </c>
       <c r="AF57" s="13">
-        <v>39012934</v>
+        <v>41349493</v>
       </c>
       <c r="AG57" s="13">
-        <v>41349493</v>
+        <v>47108405</v>
       </c>
       <c r="AH57" s="13">
-        <v>47108405</v>
+        <v>66917633</v>
       </c>
       <c r="AI57" s="13">
-        <v>66917633</v>
+        <v>55166609</v>
       </c>
       <c r="AJ57" s="13">
-        <v>55166609</v>
+        <v>67748720</v>
       </c>
       <c r="AK57" s="13">
-        <v>67748720</v>
+        <v>59311777</v>
       </c>
       <c r="AL57" s="13">
-        <v>59311777</v>
+        <v>54940072</v>
       </c>
       <c r="AM57" s="13">
-        <v>54940072</v>
+        <v>46402949</v>
       </c>
       <c r="AN57" s="13">
-        <v>46402949</v>
+        <v>70262192</v>
       </c>
       <c r="AO57" s="13">
-        <v>70262192</v>
+        <v>70040208</v>
       </c>
       <c r="AP57" s="13">
-        <v>70040208</v>
+        <v>79923483</v>
       </c>
       <c r="AQ57" s="13">
-        <v>79923483</v>
+        <v>82095147</v>
       </c>
       <c r="AR57" s="13">
-        <v>82095147</v>
+        <v>85011509</v>
       </c>
       <c r="AS57" s="13">
-        <v>85011509</v>
+        <v>92464917</v>
       </c>
       <c r="AT57" s="13">
-        <v>75597229</v>
+        <v>76634586</v>
       </c>
       <c r="AU57" s="13">
-        <v>76634586</v>
+        <v>73535970</v>
       </c>
       <c r="AV57" s="13">
-        <v>73535970</v>
+        <v>92959810</v>
       </c>
       <c r="AW57" s="13">
-        <v>92959810</v>
+        <v>109432317</v>
       </c>
       <c r="AX57" s="13">
-        <v>109432317</v>
+        <v>78161892</v>
       </c>
       <c r="AY57" s="13">
-        <v>78161892</v>
+        <v>61031662</v>
       </c>
       <c r="AZ57" s="13">
-        <v>61031662</v>
+        <v>53678996</v>
       </c>
       <c r="BA57" s="13">
-        <v>53678996</v>
+        <v>62843054</v>
       </c>
       <c r="BB57" s="13">
-        <v>62843058</v>
+        <v>64479640</v>
       </c>
     </row>
-    <row r="58" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>60</v>
       </c>
@@ -7403,95 +7368,95 @@
       <c r="Y58" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z58" s="11" t="s">
-        <v>58</v>
+      <c r="Z58" s="11">
+        <v>3397989</v>
       </c>
       <c r="AA58" s="11">
-        <v>3397989</v>
+        <v>3250810</v>
       </c>
       <c r="AB58" s="11">
-        <v>3250810</v>
+        <v>3700609</v>
       </c>
       <c r="AC58" s="11">
-        <v>3700609</v>
+        <v>5539489</v>
       </c>
       <c r="AD58" s="11">
-        <v>5539489</v>
+        <v>4381240</v>
       </c>
       <c r="AE58" s="11">
-        <v>4381240</v>
+        <v>5429270</v>
       </c>
       <c r="AF58" s="11">
-        <v>5429270</v>
+        <v>6923658</v>
       </c>
       <c r="AG58" s="11">
-        <v>6923658</v>
+        <v>5541805</v>
       </c>
       <c r="AH58" s="11">
-        <v>5541805</v>
+        <v>4949401</v>
       </c>
       <c r="AI58" s="11">
-        <v>4949401</v>
+        <v>5831556</v>
       </c>
       <c r="AJ58" s="11">
-        <v>5831556</v>
+        <v>5957563</v>
       </c>
       <c r="AK58" s="11">
-        <v>5957563</v>
+        <v>6967658</v>
       </c>
       <c r="AL58" s="11">
-        <v>6967658</v>
+        <v>6716386</v>
       </c>
       <c r="AM58" s="11">
-        <v>6716386</v>
+        <v>6605638</v>
       </c>
       <c r="AN58" s="11">
-        <v>6605638</v>
+        <v>7094069</v>
       </c>
       <c r="AO58" s="11">
-        <v>7094069</v>
+        <v>6092348</v>
       </c>
       <c r="AP58" s="11">
-        <v>6092348</v>
+        <v>7375570</v>
       </c>
       <c r="AQ58" s="11">
-        <v>7375570</v>
+        <v>7299364</v>
       </c>
       <c r="AR58" s="11">
-        <v>7299364</v>
+        <v>9414024</v>
       </c>
       <c r="AS58" s="11">
-        <v>9414024</v>
+        <v>3293161</v>
       </c>
       <c r="AT58" s="11">
-        <v>8782817</v>
+        <v>8393121</v>
       </c>
       <c r="AU58" s="11">
-        <v>8393121</v>
+        <v>7584364</v>
       </c>
       <c r="AV58" s="11">
-        <v>7584364</v>
+        <v>9291793</v>
       </c>
       <c r="AW58" s="11">
-        <v>9291793</v>
+        <v>9840810</v>
       </c>
       <c r="AX58" s="11">
-        <v>9840810</v>
+        <v>7412362</v>
       </c>
       <c r="AY58" s="11">
-        <v>7412362</v>
+        <v>6911127</v>
       </c>
       <c r="AZ58" s="11">
-        <v>6911127</v>
+        <v>6503835</v>
       </c>
       <c r="BA58" s="11">
-        <v>6503835</v>
+        <v>5654026</v>
       </c>
       <c r="BB58" s="11">
-        <v>5654026</v>
+        <v>6666641</v>
       </c>
     </row>
-    <row r="59" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B59" s="12" t="s">
         <v>61</v>
       </c>
@@ -7562,95 +7527,95 @@
       <c r="Y59" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z59" s="13" t="s">
-        <v>58</v>
+      <c r="Z59" s="13">
+        <v>12926683</v>
       </c>
       <c r="AA59" s="13">
-        <v>12926683</v>
+        <v>10609866</v>
       </c>
       <c r="AB59" s="13">
-        <v>10609866</v>
+        <v>13008132</v>
       </c>
       <c r="AC59" s="13">
-        <v>13008132</v>
+        <v>16671971</v>
       </c>
       <c r="AD59" s="13">
-        <v>16671971</v>
+        <v>14780366</v>
       </c>
       <c r="AE59" s="13">
-        <v>14780366</v>
+        <v>19914714</v>
       </c>
       <c r="AF59" s="13">
-        <v>19914714</v>
+        <v>19578474</v>
       </c>
       <c r="AG59" s="13">
-        <v>19578474</v>
+        <v>18740573</v>
       </c>
       <c r="AH59" s="13">
-        <v>18740573</v>
+        <v>21123134</v>
       </c>
       <c r="AI59" s="13">
-        <v>21123134</v>
+        <v>22195484</v>
       </c>
       <c r="AJ59" s="13">
-        <v>22195484</v>
+        <v>25120361</v>
       </c>
       <c r="AK59" s="13">
-        <v>25120361</v>
+        <v>23499295</v>
       </c>
       <c r="AL59" s="13">
-        <v>23499295</v>
+        <v>28115653</v>
       </c>
       <c r="AM59" s="13">
-        <v>28115653</v>
+        <v>27338079</v>
       </c>
       <c r="AN59" s="13">
-        <v>27338079</v>
+        <v>30934752</v>
       </c>
       <c r="AO59" s="13">
-        <v>30934752</v>
+        <v>28957328</v>
       </c>
       <c r="AP59" s="13">
-        <v>28957328</v>
+        <v>30704180</v>
       </c>
       <c r="AQ59" s="13">
-        <v>30704180</v>
+        <v>31198491</v>
       </c>
       <c r="AR59" s="13">
-        <v>31198491</v>
+        <v>27174403</v>
       </c>
       <c r="AS59" s="13">
-        <v>27174403</v>
+        <v>30372557</v>
       </c>
       <c r="AT59" s="13">
-        <v>30372557</v>
+        <v>28262693</v>
       </c>
       <c r="AU59" s="13">
-        <v>28262693</v>
+        <v>28215166</v>
       </c>
       <c r="AV59" s="13">
-        <v>28215166</v>
+        <v>29878691</v>
       </c>
       <c r="AW59" s="13">
-        <v>29878691</v>
+        <v>29328796</v>
       </c>
       <c r="AX59" s="13">
-        <v>29328796</v>
+        <v>26010864</v>
       </c>
       <c r="AY59" s="13">
-        <v>26010864</v>
+        <v>25324276</v>
       </c>
       <c r="AZ59" s="13">
-        <v>25324276</v>
+        <v>29530786</v>
       </c>
       <c r="BA59" s="13">
-        <v>29530786</v>
+        <v>28032905</v>
       </c>
       <c r="BB59" s="13">
-        <v>28032905</v>
+        <v>27105111</v>
       </c>
     </row>
-    <row r="60" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
         <v>70</v>
       </c>
@@ -7720,94 +7685,94 @@
         <v>0</v>
       </c>
       <c r="Z60" s="15">
-        <v>0</v>
+        <v>48844204</v>
       </c>
       <c r="AA60" s="15">
-        <v>48844204</v>
+        <v>42913621</v>
       </c>
       <c r="AB60" s="15">
-        <v>42913621</v>
+        <v>55101151</v>
       </c>
       <c r="AC60" s="15">
-        <v>55101151</v>
+        <v>67348088</v>
       </c>
       <c r="AD60" s="15">
-        <v>67348088</v>
+        <v>75216101</v>
       </c>
       <c r="AE60" s="15">
-        <v>75216101</v>
+        <v>78370436</v>
       </c>
       <c r="AF60" s="15">
-        <v>78370436</v>
+        <v>84724117</v>
       </c>
       <c r="AG60" s="15">
-        <v>84724117</v>
+        <v>83653566</v>
       </c>
       <c r="AH60" s="15">
-        <v>83653566</v>
+        <v>111106419</v>
       </c>
       <c r="AI60" s="15">
-        <v>111106419</v>
+        <v>90854065</v>
       </c>
       <c r="AJ60" s="15">
-        <v>90854065</v>
+        <v>124500980</v>
       </c>
       <c r="AK60" s="15">
-        <v>124500980</v>
+        <v>121298880</v>
       </c>
       <c r="AL60" s="15">
-        <v>121298880</v>
+        <v>114212036</v>
       </c>
       <c r="AM60" s="15">
-        <v>114212036</v>
+        <v>89402622</v>
       </c>
       <c r="AN60" s="15">
-        <v>89402622</v>
+        <v>120578768</v>
       </c>
       <c r="AO60" s="15">
-        <v>120578768</v>
+        <v>126484725</v>
       </c>
       <c r="AP60" s="15">
-        <v>126484725</v>
+        <v>127066952</v>
       </c>
       <c r="AQ60" s="15">
-        <v>127066952</v>
+        <v>135292297</v>
       </c>
       <c r="AR60" s="15">
-        <v>135292297</v>
+        <v>132919081</v>
       </c>
       <c r="AS60" s="15">
-        <v>132919081</v>
+        <v>126130635</v>
       </c>
       <c r="AT60" s="15">
-        <v>127470667</v>
+        <v>113290400</v>
       </c>
       <c r="AU60" s="15">
-        <v>113290400</v>
+        <v>119886041</v>
       </c>
       <c r="AV60" s="15">
-        <v>119886041</v>
+        <v>160607134</v>
       </c>
       <c r="AW60" s="15">
-        <v>160607134</v>
+        <v>169952423</v>
       </c>
       <c r="AX60" s="15">
-        <v>169952423</v>
+        <v>119741972</v>
       </c>
       <c r="AY60" s="15">
-        <v>119741972</v>
+        <v>97536544</v>
       </c>
       <c r="AZ60" s="15">
-        <v>97536544</v>
+        <v>96680666</v>
       </c>
       <c r="BA60" s="15">
-        <v>96680666</v>
+        <v>100735432</v>
       </c>
       <c r="BB60" s="15">
-        <v>100735436</v>
+        <v>102178718</v>
       </c>
     </row>
-    <row r="61" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B61" s="8" t="s">
         <v>78</v>
       </c>
@@ -7864,7 +7829,7 @@
       <c r="BA61" s="9"/>
       <c r="BB61" s="9"/>
     </row>
-    <row r="62" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B62" s="10" t="s">
         <v>56</v>
       </c>
@@ -7935,8 +7900,8 @@
       <c r="Y62" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z62" s="11" t="s">
-        <v>58</v>
+      <c r="Z62" s="11">
+        <v>0</v>
       </c>
       <c r="AA62" s="11">
         <v>0</v>
@@ -7962,8 +7927,8 @@
       <c r="AH62" s="11">
         <v>0</v>
       </c>
-      <c r="AI62" s="11">
-        <v>0</v>
+      <c r="AI62" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ62" s="11" t="s">
         <v>58</v>
@@ -7998,17 +7963,17 @@
       <c r="AT62" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AU62" s="11" t="s">
-        <v>58</v>
+      <c r="AU62" s="11">
+        <v>0</v>
       </c>
       <c r="AV62" s="11">
-        <v>0</v>
+        <v>9629688</v>
       </c>
       <c r="AW62" s="11">
-        <v>9629688</v>
+        <v>12293800</v>
       </c>
       <c r="AX62" s="11">
-        <v>12293800</v>
+        <v>0</v>
       </c>
       <c r="AY62" s="11">
         <v>0</v>
@@ -8017,13 +7982,13 @@
         <v>0</v>
       </c>
       <c r="BA62" s="11">
-        <v>0</v>
+        <v>1864834</v>
       </c>
       <c r="BB62" s="11">
-        <v>1864834</v>
+        <v>7134429</v>
       </c>
     </row>
-    <row r="63" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B63" s="12" t="s">
         <v>59</v>
       </c>
@@ -8094,8 +8059,8 @@
       <c r="Y63" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z63" s="13" t="s">
-        <v>58</v>
+      <c r="Z63" s="13">
+        <v>0</v>
       </c>
       <c r="AA63" s="13">
         <v>0</v>
@@ -8121,8 +8086,8 @@
       <c r="AH63" s="13">
         <v>0</v>
       </c>
-      <c r="AI63" s="13">
-        <v>0</v>
+      <c r="AI63" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="AJ63" s="13" t="s">
         <v>58</v>
@@ -8151,38 +8116,38 @@
       <c r="AR63" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AS63" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT63" s="13" t="s">
-        <v>58</v>
+      <c r="AS63" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT63" s="13">
+        <v>32559930</v>
       </c>
       <c r="AU63" s="13">
-        <v>32559930</v>
+        <v>516983</v>
       </c>
       <c r="AV63" s="13">
-        <v>516983</v>
+        <v>2769507</v>
       </c>
       <c r="AW63" s="13">
-        <v>2769507</v>
+        <v>4533135</v>
       </c>
       <c r="AX63" s="13">
-        <v>4533135</v>
+        <v>1725495</v>
       </c>
       <c r="AY63" s="13">
-        <v>1725495</v>
+        <v>4565522</v>
       </c>
       <c r="AZ63" s="13">
-        <v>4565522</v>
+        <v>1298496</v>
       </c>
       <c r="BA63" s="13">
-        <v>1298496</v>
+        <v>4546372</v>
       </c>
       <c r="BB63" s="13">
-        <v>4546371</v>
+        <v>4614872</v>
       </c>
     </row>
-    <row r="64" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B64" s="10" t="s">
         <v>60</v>
       </c>
@@ -8253,8 +8218,8 @@
       <c r="Y64" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z64" s="11" t="s">
-        <v>58</v>
+      <c r="Z64" s="11">
+        <v>0</v>
       </c>
       <c r="AA64" s="11">
         <v>0</v>
@@ -8280,8 +8245,8 @@
       <c r="AH64" s="11">
         <v>0</v>
       </c>
-      <c r="AI64" s="11">
-        <v>0</v>
+      <c r="AI64" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ64" s="11" t="s">
         <v>58</v>
@@ -8310,38 +8275,38 @@
       <c r="AR64" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AS64" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT64" s="11" t="s">
-        <v>58</v>
+      <c r="AS64" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT64" s="11">
+        <v>335087</v>
       </c>
       <c r="AU64" s="11">
-        <v>335087</v>
+        <v>275330</v>
       </c>
       <c r="AV64" s="11">
-        <v>275330</v>
+        <v>494149</v>
       </c>
       <c r="AW64" s="11">
-        <v>494149</v>
+        <v>536724</v>
       </c>
       <c r="AX64" s="11">
-        <v>536724</v>
+        <v>189019</v>
       </c>
       <c r="AY64" s="11">
-        <v>189019</v>
+        <v>242118</v>
       </c>
       <c r="AZ64" s="11">
-        <v>242118</v>
+        <v>85024</v>
       </c>
       <c r="BA64" s="11">
-        <v>85024</v>
+        <v>111468</v>
       </c>
       <c r="BB64" s="11">
-        <v>111468</v>
+        <v>166107</v>
       </c>
     </row>
-    <row r="65" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B65" s="12" t="s">
         <v>61</v>
       </c>
@@ -8412,8 +8377,8 @@
       <c r="Y65" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z65" s="13" t="s">
-        <v>58</v>
+      <c r="Z65" s="13">
+        <v>0</v>
       </c>
       <c r="AA65" s="13">
         <v>0</v>
@@ -8439,8 +8404,8 @@
       <c r="AH65" s="13">
         <v>0</v>
       </c>
-      <c r="AI65" s="13">
-        <v>0</v>
+      <c r="AI65" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="AJ65" s="13" t="s">
         <v>58</v>
@@ -8469,11 +8434,11 @@
       <c r="AR65" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AS65" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT65" s="13" t="s">
-        <v>58</v>
+      <c r="AS65" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT65" s="13">
+        <v>0</v>
       </c>
       <c r="AU65" s="13">
         <v>0</v>
@@ -8500,7 +8465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
         <v>72</v>
       </c>
@@ -8630,34 +8595,34 @@
         <v>0</v>
       </c>
       <c r="AT66" s="15">
-        <v>0</v>
+        <v>32895017</v>
       </c>
       <c r="AU66" s="15">
-        <v>32895017</v>
+        <v>792313</v>
       </c>
       <c r="AV66" s="15">
-        <v>792313</v>
+        <v>12893344</v>
       </c>
       <c r="AW66" s="15">
-        <v>12893344</v>
+        <v>17363659</v>
       </c>
       <c r="AX66" s="15">
-        <v>17363659</v>
+        <v>1914514</v>
       </c>
       <c r="AY66" s="15">
-        <v>1914514</v>
+        <v>4807640</v>
       </c>
       <c r="AZ66" s="15">
-        <v>4807640</v>
+        <v>1383520</v>
       </c>
       <c r="BA66" s="15">
-        <v>1383520</v>
+        <v>6522674</v>
       </c>
       <c r="BB66" s="15">
-        <v>6522673</v>
+        <v>11915408</v>
       </c>
     </row>
-    <row r="67" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>79</v>
       </c>
@@ -8714,7 +8679,7 @@
       <c r="BA67" s="9"/>
       <c r="BB67" s="9"/>
     </row>
-    <row r="68" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
         <v>56</v>
       </c>
@@ -8785,8 +8750,8 @@
       <c r="Y68" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z68" s="11" t="s">
-        <v>58</v>
+      <c r="Z68" s="11">
+        <v>0</v>
       </c>
       <c r="AA68" s="11">
         <v>0</v>
@@ -8812,8 +8777,8 @@
       <c r="AH68" s="11">
         <v>0</v>
       </c>
-      <c r="AI68" s="11">
-        <v>0</v>
+      <c r="AI68" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ68" s="11" t="s">
         <v>58</v>
@@ -8873,7 +8838,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="69" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B69" s="16" t="s">
         <v>66</v>
       </c>
@@ -8944,8 +8909,8 @@
       <c r="Y69" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Z69" s="17" t="s">
-        <v>58</v>
+      <c r="Z69" s="17">
+        <v>0</v>
       </c>
       <c r="AA69" s="17">
         <v>0</v>
@@ -9032,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B70" s="8" t="s">
         <v>80</v>
       </c>
@@ -9089,7 +9054,7 @@
       <c r="BA70" s="9"/>
       <c r="BB70" s="9"/>
     </row>
-    <row r="71" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B71" s="10" t="s">
         <v>56</v>
       </c>
@@ -9160,8 +9125,8 @@
       <c r="Y71" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z71" s="11" t="s">
-        <v>58</v>
+      <c r="Z71" s="11">
+        <v>0</v>
       </c>
       <c r="AA71" s="11">
         <v>0</v>
@@ -9187,8 +9152,8 @@
       <c r="AH71" s="11">
         <v>0</v>
       </c>
-      <c r="AI71" s="11">
-        <v>0</v>
+      <c r="AI71" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ71" s="11" t="s">
         <v>58</v>
@@ -9248,7 +9213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B72" s="16" t="s">
         <v>74</v>
       </c>
@@ -9319,8 +9284,8 @@
       <c r="Y72" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="Z72" s="17" t="s">
-        <v>58</v>
+      <c r="Z72" s="17">
+        <v>0</v>
       </c>
       <c r="AA72" s="17">
         <v>0</v>
@@ -9407,7 +9372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B73" s="8" t="s">
         <v>81</v>
       </c>
@@ -9464,7 +9429,7 @@
       <c r="BA73" s="9"/>
       <c r="BB73" s="9"/>
     </row>
-    <row r="74" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B74" s="10" t="s">
         <v>82</v>
       </c>
@@ -9535,8 +9500,8 @@
       <c r="Y74" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z74" s="11" t="s">
-        <v>58</v>
+      <c r="Z74" s="11">
+        <v>0</v>
       </c>
       <c r="AA74" s="11">
         <v>0</v>
@@ -9623,7 +9588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B75" s="16" t="s">
         <v>67</v>
       </c>
@@ -9693,94 +9658,94 @@
         <v>0</v>
       </c>
       <c r="Z75" s="17">
-        <v>0</v>
+        <v>48844204</v>
       </c>
       <c r="AA75" s="17">
-        <v>48844204</v>
+        <v>42913621</v>
       </c>
       <c r="AB75" s="17">
-        <v>42913621</v>
+        <v>55101151</v>
       </c>
       <c r="AC75" s="17">
-        <v>55101151</v>
+        <v>67348088</v>
       </c>
       <c r="AD75" s="17">
-        <v>67348088</v>
+        <v>75216101</v>
       </c>
       <c r="AE75" s="17">
-        <v>75216101</v>
+        <v>78370436</v>
       </c>
       <c r="AF75" s="17">
-        <v>78370436</v>
+        <v>84724117</v>
       </c>
       <c r="AG75" s="17">
-        <v>84724117</v>
+        <v>83653566</v>
       </c>
       <c r="AH75" s="17">
-        <v>83653566</v>
+        <v>111106419</v>
       </c>
       <c r="AI75" s="17">
-        <v>111106419</v>
+        <v>90854065</v>
       </c>
       <c r="AJ75" s="17">
-        <v>90854065</v>
+        <v>124500980</v>
       </c>
       <c r="AK75" s="17">
-        <v>124500980</v>
+        <v>121298880</v>
       </c>
       <c r="AL75" s="17">
-        <v>121298880</v>
+        <v>114212036</v>
       </c>
       <c r="AM75" s="17">
-        <v>114212036</v>
+        <v>89402622</v>
       </c>
       <c r="AN75" s="17">
-        <v>89402622</v>
+        <v>120578768</v>
       </c>
       <c r="AO75" s="17">
-        <v>120578768</v>
+        <v>126484725</v>
       </c>
       <c r="AP75" s="17">
-        <v>126484725</v>
+        <v>127066952</v>
       </c>
       <c r="AQ75" s="17">
-        <v>127066952</v>
+        <v>135292297</v>
       </c>
       <c r="AR75" s="17">
-        <v>135292297</v>
+        <v>132919081</v>
       </c>
       <c r="AS75" s="17">
-        <v>132919081</v>
+        <v>126130635</v>
       </c>
       <c r="AT75" s="17">
-        <v>127470667</v>
+        <v>146185417</v>
       </c>
       <c r="AU75" s="17">
-        <v>146185417</v>
+        <v>120678354</v>
       </c>
       <c r="AV75" s="17">
-        <v>120678354</v>
+        <v>173500478</v>
       </c>
       <c r="AW75" s="17">
-        <v>173500478</v>
+        <v>187316082</v>
       </c>
       <c r="AX75" s="17">
-        <v>187316082</v>
+        <v>121656486</v>
       </c>
       <c r="AY75" s="17">
-        <v>121656486</v>
+        <v>102344184</v>
       </c>
       <c r="AZ75" s="17">
-        <v>102344184</v>
+        <v>98064186</v>
       </c>
       <c r="BA75" s="17">
-        <v>98064186</v>
+        <v>107258106</v>
       </c>
       <c r="BB75" s="17">
-        <v>107258109</v>
+        <v>114094126</v>
       </c>
     </row>
-    <row r="76" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -9835,7 +9800,7 @@
       <c r="BA76" s="1"/>
       <c r="BB76" s="1"/>
     </row>
-    <row r="77" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -9890,7 +9855,7 @@
       <c r="BA77" s="1"/>
       <c r="BB77" s="1"/>
     </row>
-    <row r="78" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -9945,7 +9910,7 @@
       <c r="BA78" s="1"/>
       <c r="BB78" s="1"/>
     </row>
-    <row r="79" spans="2:54" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:54" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B79" s="7" t="s">
         <v>83</v>
       </c>
@@ -10102,7 +10067,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="80" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -10157,7 +10122,7 @@
       <c r="BA80" s="1"/>
       <c r="BB80" s="1"/>
     </row>
-    <row r="81" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B81" s="8" t="s">
         <v>84</v>
       </c>
@@ -10214,7 +10179,7 @@
       <c r="BA81" s="9"/>
       <c r="BB81" s="9"/>
     </row>
-    <row r="82" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="s">
         <v>56</v>
       </c>
@@ -10285,95 +10250,95 @@
       <c r="Y82" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z82" s="11" t="s">
-        <v>58</v>
+      <c r="Z82" s="11">
+        <v>59631872000</v>
       </c>
       <c r="AA82" s="11">
-        <v>59631872000</v>
+        <v>79758161290</v>
       </c>
       <c r="AB82" s="11">
-        <v>79758161290</v>
+        <v>74270857143</v>
       </c>
       <c r="AC82" s="11">
-        <v>74270857143</v>
+        <v>94046065217</v>
       </c>
       <c r="AD82" s="11">
-        <v>94046065217</v>
+        <v>95832156977</v>
       </c>
       <c r="AE82" s="11">
-        <v>95832156977</v>
+        <v>114864901639</v>
       </c>
       <c r="AF82" s="11">
-        <v>114864901639</v>
+        <v>123156875912</v>
       </c>
       <c r="AG82" s="11">
-        <v>123156875912</v>
+        <v>121413693069</v>
       </c>
       <c r="AH82" s="11">
-        <v>121413693069</v>
+        <v>131277181159</v>
       </c>
       <c r="AI82" s="11">
-        <v>131277181159</v>
+        <v>136793142857</v>
       </c>
       <c r="AJ82" s="11">
-        <v>136793142857</v>
+        <v>134420607330</v>
       </c>
       <c r="AK82" s="11">
-        <v>134420607330</v>
+        <v>135279613734</v>
       </c>
       <c r="AL82" s="11">
-        <v>135279613734</v>
+        <v>153710220126</v>
       </c>
       <c r="AM82" s="11">
-        <v>153710220126</v>
+        <v>153490779661</v>
       </c>
       <c r="AN82" s="11">
-        <v>153490779661</v>
+        <v>153596937500</v>
       </c>
       <c r="AO82" s="11">
-        <v>153596937500</v>
+        <v>165851480620</v>
       </c>
       <c r="AP82" s="11">
-        <v>165851480620</v>
+        <v>146189016129</v>
       </c>
       <c r="AQ82" s="11">
-        <v>146189016129</v>
+        <v>161530714286</v>
       </c>
       <c r="AR82" s="11">
-        <v>161530714286</v>
-      </c>
-      <c r="AS82" s="11">
         <v>164045579710</v>
       </c>
-      <c r="AT82" s="11">
-        <v>151405523810</v>
-      </c>
-      <c r="AU82" s="11" t="s">
-        <v>58</v>
+      <c r="AS82" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT82" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU82" s="11">
+        <v>157470761194</v>
       </c>
       <c r="AV82" s="11">
-        <v>157470761194</v>
+        <v>165467545671</v>
       </c>
       <c r="AW82" s="11">
-        <v>165467545671</v>
+        <v>166800786338</v>
       </c>
       <c r="AX82" s="11">
-        <v>166800786338</v>
+        <v>181408972892</v>
       </c>
       <c r="AY82" s="11">
-        <v>181408972892</v>
+        <v>147223413793</v>
       </c>
       <c r="AZ82" s="11">
-        <v>147223413793</v>
+        <v>154823311111</v>
       </c>
       <c r="BA82" s="11">
-        <v>154823311111</v>
+        <v>182845521739</v>
       </c>
       <c r="BB82" s="11">
-        <v>182845521739</v>
+        <v>151051000000</v>
       </c>
     </row>
-    <row r="83" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B83" s="12" t="s">
         <v>59</v>
       </c>
@@ -10444,95 +10409,95 @@
       <c r="Y83" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z83" s="13" t="s">
-        <v>58</v>
+      <c r="Z83" s="13">
+        <v>67020181818</v>
       </c>
       <c r="AA83" s="13">
-        <v>67020181818</v>
+        <v>74637582043</v>
       </c>
       <c r="AB83" s="13">
-        <v>74637582043</v>
+        <v>82870252577</v>
       </c>
       <c r="AC83" s="13">
-        <v>82870252577</v>
+        <v>95011432292</v>
       </c>
       <c r="AD83" s="13">
-        <v>95011432292</v>
+        <v>108414695890</v>
       </c>
       <c r="AE83" s="13">
-        <v>108414695890</v>
+        <v>121158180124</v>
       </c>
       <c r="AF83" s="13">
-        <v>121158180124</v>
+        <v>126838935583</v>
       </c>
       <c r="AG83" s="13">
-        <v>126838935583</v>
+        <v>131221183844</v>
       </c>
       <c r="AH83" s="13">
-        <v>131221183844</v>
+        <v>147395667401</v>
       </c>
       <c r="AI83" s="13">
-        <v>147395667401</v>
+        <v>165169488024</v>
       </c>
       <c r="AJ83" s="13">
-        <v>165169488024</v>
+        <v>171515746835</v>
       </c>
       <c r="AK83" s="13">
-        <v>171515746835</v>
+        <v>177050080597</v>
       </c>
       <c r="AL83" s="13">
-        <v>177050080597</v>
+        <v>182525156146</v>
       </c>
       <c r="AM83" s="13">
-        <v>182525156146</v>
+        <v>196622665254</v>
       </c>
       <c r="AN83" s="13">
-        <v>196622665254</v>
+        <v>206047483871</v>
       </c>
       <c r="AO83" s="13">
-        <v>206047483871</v>
+        <v>209075247761</v>
       </c>
       <c r="AP83" s="13">
-        <v>209075247761</v>
+        <v>214848072581</v>
       </c>
       <c r="AQ83" s="13">
-        <v>214848072581</v>
+        <v>209962012788</v>
       </c>
       <c r="AR83" s="13">
-        <v>209962012788</v>
+        <v>213596756281</v>
       </c>
       <c r="AS83" s="13">
-        <v>213596756281</v>
+        <v>199401770724</v>
       </c>
       <c r="AT83" s="13">
-        <v>205427252717</v>
+        <v>191586465000</v>
       </c>
       <c r="AU83" s="13">
-        <v>191586465000</v>
+        <v>198210161725</v>
       </c>
       <c r="AV83" s="13">
-        <v>198210161725</v>
+        <v>202526819172</v>
       </c>
       <c r="AW83" s="13">
-        <v>202526819172</v>
+        <v>209239611855</v>
       </c>
       <c r="AX83" s="13">
-        <v>209239611855</v>
+        <v>201162924842</v>
       </c>
       <c r="AY83" s="13">
-        <v>201162924842</v>
+        <v>193751307937</v>
       </c>
       <c r="AZ83" s="13">
-        <v>193751307937</v>
+        <v>180737360269</v>
       </c>
       <c r="BA83" s="13">
-        <v>180737360269</v>
+        <v>175122663243</v>
       </c>
       <c r="BB83" s="13">
-        <v>175050300836</v>
+        <v>169683263158</v>
       </c>
     </row>
-    <row r="84" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B84" s="10" t="s">
         <v>60</v>
       </c>
@@ -10603,95 +10568,95 @@
       <c r="Y84" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z84" s="11" t="s">
-        <v>58</v>
+      <c r="Z84" s="11">
+        <v>121356750000</v>
       </c>
       <c r="AA84" s="11">
-        <v>121356750000</v>
+        <v>120400370370</v>
       </c>
       <c r="AB84" s="11">
-        <v>120400370370</v>
+        <v>137059592593</v>
       </c>
       <c r="AC84" s="11">
-        <v>137059592593</v>
+        <v>145776026316</v>
       </c>
       <c r="AD84" s="11">
-        <v>145776026316</v>
+        <v>175249600000</v>
       </c>
       <c r="AE84" s="11">
-        <v>175249600000</v>
+        <v>187216206897</v>
       </c>
       <c r="AF84" s="11">
-        <v>187216206897</v>
+        <v>187125891892</v>
       </c>
       <c r="AG84" s="11">
-        <v>187125891892</v>
+        <v>221672200000</v>
       </c>
       <c r="AH84" s="11">
-        <v>221672200000</v>
+        <v>224972772727</v>
       </c>
       <c r="AI84" s="11">
-        <v>224972772727</v>
+        <v>233262240000</v>
       </c>
       <c r="AJ84" s="11">
-        <v>233262240000</v>
+        <v>229137038462</v>
       </c>
       <c r="AK84" s="11">
-        <v>229137038462</v>
+        <v>240264068966</v>
       </c>
       <c r="AL84" s="11">
-        <v>240264068966</v>
+        <v>248755037037</v>
       </c>
       <c r="AM84" s="11">
-        <v>248755037037</v>
+        <v>264225520000</v>
       </c>
       <c r="AN84" s="11">
-        <v>264225520000</v>
+        <v>283762760000</v>
       </c>
       <c r="AO84" s="11">
-        <v>283762760000</v>
+        <v>304617400000</v>
       </c>
       <c r="AP84" s="11">
-        <v>304617400000</v>
+        <v>295022800000</v>
       </c>
       <c r="AQ84" s="11">
-        <v>295022800000</v>
+        <v>291974560000</v>
       </c>
       <c r="AR84" s="11">
-        <v>291974560000</v>
+        <v>294188250000</v>
       </c>
       <c r="AS84" s="11">
-        <v>294188250000</v>
+        <v>299670260531</v>
       </c>
       <c r="AT84" s="11">
-        <v>292760566667</v>
+        <v>289417965517</v>
       </c>
       <c r="AU84" s="11">
-        <v>289417965517</v>
+        <v>316015166667</v>
       </c>
       <c r="AV84" s="11">
-        <v>316015166667</v>
+        <v>309726433333</v>
       </c>
       <c r="AW84" s="11">
-        <v>309726433333</v>
+        <v>289435588235</v>
       </c>
       <c r="AX84" s="11">
-        <v>289435588235</v>
+        <v>311586494932</v>
       </c>
       <c r="AY84" s="11">
-        <v>311586494932</v>
+        <v>300483782609</v>
       </c>
       <c r="AZ84" s="11">
-        <v>300483782609</v>
+        <v>295628863636</v>
       </c>
       <c r="BA84" s="11">
-        <v>295628863636</v>
+        <v>314112555556</v>
       </c>
       <c r="BB84" s="11">
-        <v>314112555556</v>
+        <v>303029136364</v>
       </c>
     </row>
-    <row r="85" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B85" s="12" t="s">
         <v>61</v>
       </c>
@@ -10762,95 +10727,95 @@
       <c r="Y85" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="Z85" s="13" t="s">
-        <v>58</v>
+      <c r="Z85" s="13">
+        <v>86756261745</v>
       </c>
       <c r="AA85" s="13">
-        <v>86756261745</v>
+        <v>93892619469</v>
       </c>
       <c r="AB85" s="13">
-        <v>93892619469</v>
+        <v>108401100000</v>
       </c>
       <c r="AC85" s="13">
-        <v>108401100000</v>
+        <v>126302810606</v>
       </c>
       <c r="AD85" s="13">
-        <v>126302810606</v>
+        <v>134366963636</v>
       </c>
       <c r="AE85" s="13">
-        <v>134366963636</v>
+        <v>146431720588</v>
       </c>
       <c r="AF85" s="13">
-        <v>146431720588</v>
+        <v>156627792000</v>
       </c>
       <c r="AG85" s="13">
-        <v>156627792000</v>
+        <v>167326544643</v>
       </c>
       <c r="AH85" s="13">
-        <v>167326544643</v>
+        <v>180539606838</v>
       </c>
       <c r="AI85" s="13">
-        <v>180539606838</v>
+        <v>194697228070</v>
       </c>
       <c r="AJ85" s="13">
-        <v>194697228070</v>
+        <v>200962888000</v>
       </c>
       <c r="AK85" s="13">
-        <v>200962888000</v>
+        <v>207958362832</v>
       </c>
       <c r="AL85" s="13">
-        <v>207958362832</v>
+        <v>224925224000</v>
       </c>
       <c r="AM85" s="13">
-        <v>224925224000</v>
+        <v>233658794872</v>
       </c>
       <c r="AN85" s="13">
-        <v>233658794872</v>
+        <v>239804279070</v>
       </c>
       <c r="AO85" s="13">
-        <v>239804279070</v>
+        <v>241311066667</v>
       </c>
       <c r="AP85" s="13">
-        <v>241311066667</v>
+        <v>241765196850</v>
       </c>
       <c r="AQ85" s="13">
-        <v>241765196850</v>
+        <v>239988392308</v>
       </c>
       <c r="AR85" s="13">
-        <v>239988392308</v>
+        <v>242628598214</v>
       </c>
       <c r="AS85" s="13">
-        <v>242628598214</v>
+        <v>242638527098</v>
       </c>
       <c r="AT85" s="13">
-        <v>242980456000</v>
+        <v>235522441667</v>
       </c>
       <c r="AU85" s="13">
-        <v>235522441667</v>
+        <v>235126383333</v>
       </c>
       <c r="AV85" s="13">
-        <v>235126383333</v>
+        <v>228081610687</v>
       </c>
       <c r="AW85" s="13">
-        <v>228081610687</v>
+        <v>229131218750</v>
       </c>
       <c r="AX85" s="13">
-        <v>229131218750</v>
+        <v>231300256339</v>
       </c>
       <c r="AY85" s="13">
-        <v>231300256339</v>
+        <v>234484037037</v>
       </c>
       <c r="AZ85" s="13">
-        <v>234484037037</v>
+        <v>230709265625</v>
       </c>
       <c r="BA85" s="13">
-        <v>230709265625</v>
+        <v>229777909836</v>
       </c>
       <c r="BB85" s="13">
-        <v>229777909836</v>
+        <v>229704330508</v>
       </c>
     </row>
-    <row r="86" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>86</v>
       </c>
@@ -10907,7 +10872,7 @@
       <c r="BA86" s="9"/>
       <c r="BB86" s="9"/>
     </row>
-    <row r="87" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="s">
         <v>56</v>
       </c>
@@ -11044,29 +11009,29 @@
       <c r="AU87" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AV87" s="11" t="s">
-        <v>58</v>
+      <c r="AV87" s="11">
+        <v>137566971429</v>
       </c>
       <c r="AW87" s="11">
-        <v>137566971429</v>
+        <v>147187612736</v>
       </c>
       <c r="AX87" s="11">
-        <v>147187612736</v>
-      </c>
-      <c r="AY87" s="11">
-        <v>0</v>
-      </c>
-      <c r="AZ87" s="11" t="s">
-        <v>58</v>
+        <v>0</v>
+      </c>
+      <c r="AY87" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="AZ87" s="11">
+        <v>0</v>
       </c>
       <c r="BA87" s="11">
-        <v>0</v>
+        <v>124322266667</v>
       </c>
       <c r="BB87" s="11">
-        <v>124322266667</v>
+        <v>118907150000</v>
       </c>
     </row>
-    <row r="88" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B88" s="12" t="s">
         <v>59</v>
       </c>
@@ -11194,38 +11159,38 @@
       <c r="AR88" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="AS88" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT88" s="13" t="s">
-        <v>58</v>
+      <c r="AS88" s="13">
+        <v>0</v>
+      </c>
+      <c r="AT88" s="13">
+        <v>143435814978</v>
       </c>
       <c r="AU88" s="13">
-        <v>143435814978</v>
+        <v>258491500000</v>
       </c>
       <c r="AV88" s="13">
-        <v>258491500000</v>
+        <v>230792250000</v>
       </c>
       <c r="AW88" s="13">
-        <v>230792250000</v>
+        <v>238586030303</v>
       </c>
       <c r="AX88" s="13">
-        <v>238586030303</v>
+        <v>215686875000</v>
       </c>
       <c r="AY88" s="13">
-        <v>215686875000</v>
+        <v>228276100000</v>
       </c>
       <c r="AZ88" s="13">
-        <v>228276100000</v>
+        <v>185499428571</v>
       </c>
       <c r="BA88" s="13">
-        <v>185499428571</v>
+        <v>166196017471</v>
       </c>
       <c r="BB88" s="13">
-        <v>168384111111</v>
+        <v>177495076923</v>
       </c>
     </row>
-    <row r="89" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B89" s="10" t="s">
         <v>60</v>
       </c>
@@ -11353,38 +11318,38 @@
       <c r="AR89" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AS89" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="AT89" s="11" t="s">
-        <v>58</v>
+      <c r="AS89" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT89" s="11">
+        <v>335087000000</v>
       </c>
       <c r="AU89" s="11">
-        <v>335087000000</v>
+        <v>275330000000</v>
       </c>
       <c r="AV89" s="11">
-        <v>275330000000</v>
+        <v>247074500000</v>
       </c>
       <c r="AW89" s="11">
-        <v>247074500000</v>
+        <v>268362000000</v>
       </c>
       <c r="AX89" s="11">
-        <v>268362000000</v>
+        <v>189019000000</v>
       </c>
       <c r="AY89" s="11">
-        <v>189019000000</v>
+        <v>242118000000</v>
       </c>
       <c r="AZ89" s="11">
-        <v>242118000000</v>
+        <v>0</v>
       </c>
       <c r="BA89" s="11">
         <v>0</v>
       </c>
-      <c r="BB89" s="11" t="s">
-        <v>58</v>
+      <c r="BB89" s="11">
+        <v>166107000000</v>
       </c>
     </row>
-    <row r="90" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B90" s="8" t="s">
         <v>87</v>
       </c>
@@ -11441,7 +11406,7 @@
       <c r="BA90" s="9"/>
       <c r="BB90" s="9"/>
     </row>
-    <row r="91" spans="2:54" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B91" s="10" t="s">
         <v>56</v>
       </c>
@@ -11512,8 +11477,8 @@
       <c r="Y91" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Z91" s="11" t="s">
-        <v>58</v>
+      <c r="Z91" s="11">
+        <v>0</v>
       </c>
       <c r="AA91" s="11">
         <v>0</v>
@@ -11539,8 +11504,8 @@
       <c r="AH91" s="11">
         <v>0</v>
       </c>
-      <c r="AI91" s="11">
-        <v>0</v>
+      <c r="AI91" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="AJ91" s="11" t="s">
         <v>58</v>

</xml_diff>